<commit_message>
RDM-3317 - merged with master
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V39_RDM-3317.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V39_RDM-3317.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\moj\ccd-definition-store-api\application\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3917D685-B88B-4E98-8332-6B15C1C0ED54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6850E843-D54F-446E-89FA-9F111DABB7BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2860" windowWidth="28800" windowHeight="16780" tabRatio="726" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2260" windowWidth="28800" windowHeight="16780" tabRatio="500" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,12 @@
     <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
-    <sheet name="SearchAlias" sheetId="21" r:id="rId20"/>
+    <sheet name="SearchAlias" sheetId="22" r:id="rId20"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId21"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="328">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1010,6 +1010,24 @@
   </si>
   <si>
     <t>LegacyCase FirstName Hint Override</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>referenceCollection</t>
+  </si>
+  <si>
+    <t>Reference Collection</t>
+  </si>
+  <si>
+    <t>MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>#TABLE(Title, FirstName, MiddleName)</t>
+  </si>
+  <si>
+    <t>ReferenceCollectionTab</t>
   </si>
   <si>
     <t>SearchAlias</t>
@@ -1042,7 +1060,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1310,6 +1328,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1567,7 +1597,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1781,6 +1811,14 @@
     <xf numFmtId="49" fontId="39" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="26" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="22" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="23" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2201,7 +2239,7 @@
   <cols>
     <col min="1" max="1" width="17.17578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.29296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.17578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="43.8203125" style="1" customWidth="1"/>
     <col min="6" max="10" width="8.8203125" style="1" customWidth="1"/>
@@ -2429,8 +2467,8 @@
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.8203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.17578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.29296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.64453125" style="1" customWidth="1"/>
     <col min="7" max="11" width="8.8203125" style="1" customWidth="1"/>
     <col min="12" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -2794,11 +2832,11 @@
     <col min="3" max="3" width="29.8203125" style="57" customWidth="1"/>
     <col min="4" max="4" width="19.8203125" style="57" customWidth="1"/>
     <col min="5" max="5" width="20.17578125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="15.29296875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="15.3515625" style="57" customWidth="1"/>
     <col min="7" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="58" t="s">
         <v>219</v>
       </c>
@@ -3105,10 +3143,10 @@
   <cols>
     <col min="1" max="1" width="34.46875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.29296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.3515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.46875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.29296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.64453125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
     <col min="8" max="11" width="8.8203125" style="1" customWidth="1"/>
     <col min="12" max="1025" width="8.8203125" customWidth="1"/>
@@ -3460,10 +3498,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -3471,13 +3509,13 @@
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.8203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.8203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.64453125" style="1" customWidth="1"/>
     <col min="5" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.29296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="40.8203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.29296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.29296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.3515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.3515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="8.8203125" style="1" customWidth="1"/>
     <col min="15" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -3536,7 +3574,9 @@
       <c r="K2" s="105" t="s">
         <v>271</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="L2" s="157" t="s">
+        <v>318</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
@@ -3574,7 +3614,9 @@
       <c r="K3" s="106" t="s">
         <v>268</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="159" t="s">
+        <v>315</v>
+      </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
@@ -3716,31 +3758,33 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>233</v>
+      <c r="E8" s="122" t="s">
+        <v>320</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>10</v>
+        <v>317</v>
       </c>
       <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="H8" s="161" t="s">
+        <v>316</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="162" t="s">
+        <v>319</v>
+      </c>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
     </row>
     <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="9">
@@ -3763,10 +3807,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -3786,19 +3830,19 @@
         <v>232</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="4">
         <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -3818,16 +3862,16 @@
         <v>232</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>235</v>
+        <v>55</v>
       </c>
       <c r="G11" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="I11" s="4">
         <v>1</v>
@@ -3850,7 +3894,7 @@
         <v>232</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F12" s="53" t="s">
         <v>235</v>
@@ -3859,10 +3903,10 @@
         <v>3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I12" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -3882,7 +3926,7 @@
         <v>232</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F13" s="53" t="s">
         <v>235</v>
@@ -3891,10 +3935,10 @@
         <v>3</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I13" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -3914,19 +3958,19 @@
         <v>232</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G14" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I14" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -3946,19 +3990,19 @@
         <v>232</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G15" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I15" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -3978,7 +4022,7 @@
         <v>232</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F16" s="53" t="s">
         <v>235</v>
@@ -3987,10 +4031,10 @@
         <v>3</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I16" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -4010,7 +4054,7 @@
         <v>232</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17" s="53" t="s">
         <v>235</v>
@@ -4019,10 +4063,10 @@
         <v>3</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -4030,16 +4074,32 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="9">
+        <v>42736</v>
+      </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="4">
+        <v>6</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -4189,6 +4249,22 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -4211,7 +4287,7 @@
   <cols>
     <col min="1" max="1" width="16.17578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.8203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.29296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.3515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.46875" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.8203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.8203125" style="1" customWidth="1"/>
@@ -4420,7 +4496,7 @@
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="27.8203125" style="119" customWidth="1"/>
-    <col min="2" max="2" width="24.703125" style="119" customWidth="1"/>
+    <col min="2" max="2" width="24.64453125" style="119" customWidth="1"/>
     <col min="3" max="3" width="30" style="119" customWidth="1"/>
     <col min="4" max="4" width="27.17578125" style="119" customWidth="1"/>
     <col min="5" max="5" width="23.8203125" style="119" customWidth="1"/>
@@ -4569,9 +4645,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.64453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.29296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.8203125" style="1" customWidth="1"/>
     <col min="5" max="250" width="14.46875" style="1" customWidth="1"/>
     <col min="251" max="1020" width="8.8203125" customWidth="1"/>
@@ -4837,7 +4913,7 @@
       <c r="IO1" s="17"/>
       <c r="IP1" s="17"/>
     </row>
-    <row r="2" spans="1:250" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:250" ht="65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="132"/>
       <c r="B2" s="132"/>
       <c r="C2" s="133" t="s">
@@ -7710,10 +7786,10 @@
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.29296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.17578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.46875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.29296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.3515625" style="1" customWidth="1"/>
     <col min="7" max="1019" width="8.8203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7733,7 +7809,7 @@
       <c r="E1" s="136"/>
       <c r="F1" s="136"/>
     </row>
-    <row r="2" spans="1:6" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="137"/>
       <c r="B2" s="137"/>
       <c r="C2" s="138" t="s">
@@ -8290,10 +8366,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.29296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.3515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.8203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.64453125" style="1" customWidth="1"/>
     <col min="5" max="255" width="14.46875" style="1" customWidth="1"/>
     <col min="256" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -8563,7 +8639,7 @@
       <c r="IT1" s="23"/>
       <c r="IU1" s="24"/>
     </row>
-    <row r="2" spans="1:255" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:255" ht="65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -12323,7 +12399,7 @@
     <col min="1" max="1" width="28.17578125" style="81" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="81" customWidth="1"/>
     <col min="3" max="3" width="27.8203125" style="81" customWidth="1"/>
-    <col min="4" max="4" width="18.703125" style="81" customWidth="1"/>
+    <col min="4" max="4" width="18.64453125" style="81" customWidth="1"/>
     <col min="5" max="255" width="14.46875" style="81" customWidth="1"/>
     <col min="256" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -12593,7 +12669,7 @@
       <c r="IT1" s="88"/>
       <c r="IU1" s="89"/>
     </row>
-    <row r="2" spans="1:255" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:255" ht="65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="90"/>
       <c r="B2" s="90"/>
       <c r="C2" s="91" t="s">
@@ -13209,9 +13285,9 @@
     <col min="3" max="3" width="27.8203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="31.8203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.8203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.29296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.8203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.29296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="14" width="8.8203125" style="1" customWidth="1"/>
     <col min="15" max="1025" width="8.8203125" customWidth="1"/>
@@ -13241,7 +13317,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" ht="74" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -13563,106 +13639,104 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80593354-9804-4DA6-8127-5582F3E20BDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E894500-2813-4F1B-AF33-45976615BC25}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="25.703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.52734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.29296875" customWidth="1"/>
-    <col min="4" max="4" width="15.17578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="157" t="s">
-        <v>315</v>
-      </c>
-      <c r="B1" s="158" t="s">
+      <c r="A1" s="163" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="159" t="s">
+      <c r="C1" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="160" t="s">
+      <c r="D1" s="166" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="50.7" x14ac:dyDescent="0.4">
-      <c r="A2" s="161"/>
-      <c r="B2" s="161" t="s">
-        <v>316</v>
-      </c>
-      <c r="C2" s="161" t="s">
-        <v>317</v>
-      </c>
-      <c r="D2" s="161"/>
+    <row r="2" spans="1:4" ht="76" x14ac:dyDescent="0.4">
+      <c r="A2" s="167"/>
+      <c r="B2" s="167" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="167" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" s="167"/>
     </row>
     <row r="3" spans="1:4" ht="14.35" x14ac:dyDescent="0.5">
-      <c r="A3" s="162" t="s">
+      <c r="A3" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="162" t="s">
-        <v>318</v>
-      </c>
-      <c r="C3" s="162" t="s">
+      <c r="B3" s="168" t="s">
+        <v>324</v>
+      </c>
+      <c r="C3" s="168" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="162"/>
+      <c r="D3" s="168"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="163" t="s">
+      <c r="A4" s="169" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="130" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C4" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="164"/>
+      <c r="D4" s="170"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="163" t="s">
+      <c r="A5" s="169" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="130" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C5" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="164"/>
+      <c r="D5" s="170"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="169" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="164" t="s">
-        <v>320</v>
+      <c r="B6" s="170" t="s">
+        <v>326</v>
       </c>
       <c r="C6" s="130" t="s">
-        <v>321</v>
-      </c>
-      <c r="D6" s="164"/>
+        <v>327</v>
+      </c>
+      <c r="D6" s="170"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="164"/>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
+      <c r="A7" s="170"/>
+      <c r="B7" s="170"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{5E4D8216-235E-4664-BD66-A77F2ABDF7AD}">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{74390B4F-92B1-4E3B-B140-E37519C73749}">
           <x14:formula1>
             <xm:f>[CCD_TestDefinition.xlsx]CaseType!#REF!</xm:f>
           </x14:formula1>
@@ -13679,10 +13753,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="92" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -13695,7 +13769,7 @@
     <col min="6" max="6" width="24.8203125" style="1" customWidth="1"/>
     <col min="7" max="8" width="37" style="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.29296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.3515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
     <col min="12" max="18" width="8.8203125" style="1" customWidth="1"/>
     <col min="19" max="23" width="14.46875" style="1" customWidth="1"/>
@@ -14289,25 +14363,25 @@
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="D16" s="122" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" s="122" t="s">
+        <v>317</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="H16" s="122" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -14331,10 +14405,10 @@
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="3" t="s">
@@ -14346,7 +14420,7 @@
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -14370,20 +14444,22 @@
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -14407,14 +14483,14 @@
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -14444,20 +14520,20 @@
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -14481,14 +14557,14 @@
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -14518,20 +14594,20 @@
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -14555,20 +14631,20 @@
         <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -14592,20 +14668,20 @@
         <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="3" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -14629,22 +14705,20 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -14668,22 +14742,22 @@
         <v>27</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -14707,22 +14781,22 @@
         <v>27</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -14746,22 +14820,22 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -14777,17 +14851,31 @@
       <c r="W28" s="26"/>
     </row>
     <row r="29" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="9"/>
+      <c r="A29" s="9">
+        <v>42736</v>
+      </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="G29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -15020,11 +15108,36 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="35"/>
-      <c r="T38" s="36"/>
-      <c r="U38" s="36"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="37"/>
+      <c r="S38" s="25"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="26"/>
+    </row>
+    <row r="39" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="36"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -15045,8 +15158,8 @@
   <cols>
     <col min="1" max="1" width="15.17578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="31.703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.29296875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="31.64453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.3515625" style="1" customWidth="1"/>
     <col min="6" max="10" width="8.8203125" style="1" customWidth="1"/>
     <col min="11" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -15384,20 +15497,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.64453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.46875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.46875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.64453125" style="1" customWidth="1"/>
     <col min="6" max="7" width="21.46875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.8203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.29296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.17578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.64453125" style="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="1" customWidth="1"/>
     <col min="13" max="19" width="8.8203125" style="1" customWidth="1"/>
     <col min="20" max="1025" width="8.8203125" customWidth="1"/>
@@ -16314,13 +16429,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.29296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.8203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.46875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.64453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.64453125" style="1" customWidth="1"/>
     <col min="8" max="12" width="8.8203125" style="1" customWidth="1"/>
     <col min="13" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -16694,26 +16809,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.64453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.8203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.64453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.64453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="45.46875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.64453125" style="1" customWidth="1"/>
     <col min="8" max="8" width="45.46875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.64453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.64453125" style="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="1" customWidth="1"/>
     <col min="12" max="12" width="31.46875" style="1" customWidth="1"/>
     <col min="13" max="13" width="29.8203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.29296875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.64453125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.3515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.64453125" style="1" customWidth="1"/>
     <col min="17" max="17" width="31.17578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="8.8203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.64453125" style="1" customWidth="1"/>
     <col min="21" max="21" width="8.8203125" style="1" customWidth="1"/>
     <col min="22" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
@@ -16749,7 +16864,7 @@
       <c r="T1" s="101"/>
       <c r="U1" s="4"/>
     </row>
-    <row r="2" spans="1:21" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -17384,32 +17499,32 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.64453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.64453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.64453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.46875" style="1" customWidth="1"/>
     <col min="7" max="8" width="17.8203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.46875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="20.17578125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="22" style="1" customWidth="1"/>
-    <col min="14" max="14" width="45.29296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="34.29296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.9375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="1024" width="8.8203125" customWidth="1"/>
+    <col min="10" max="12" width="20.17578125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="22" style="1" customWidth="1"/>
+    <col min="15" max="15" width="45.3515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="34.3515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.64453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -17429,14 +17544,15 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="101"/>
-      <c r="L1" s="4"/>
+      <c r="L1" s="101"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -17464,22 +17580,23 @@
       <c r="K2" s="102" t="s">
         <v>264</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="158"/>
+      <c r="M2" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="O2" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="O2" s="107" t="s">
+      <c r="P2" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
-    </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -17513,26 +17630,29 @@
       <c r="K3" s="103" t="s">
         <v>265</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="159" t="s">
+        <v>315</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="P3" s="156" t="s">
+      <c r="Q3" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="Q3" s="156" t="s">
+      <c r="R3" s="156" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -17562,22 +17682,23 @@
       <c r="K4" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="101"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>2</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -17607,16 +17728,17 @@
       <c r="K5" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="101"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4">
+      <c r="O5" s="4"/>
+      <c r="P5" s="4">
         <v>1</v>
       </c>
-      <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -17646,16 +17768,17 @@
       <c r="K6" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="101"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -17681,16 +17804,17 @@
       <c r="K7" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="101"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4"/>
+      <c r="O7" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -17716,16 +17840,17 @@
       <c r="K8" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="101"/>
+      <c r="M8" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4"/>
+      <c r="N8" s="3"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -17755,14 +17880,15 @@
       <c r="K9" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="101"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="3"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="114">
         <v>42736</v>
       </c>
@@ -17794,14 +17920,15 @@
       </c>
       <c r="L10" s="118"/>
       <c r="M10" s="118"/>
-      <c r="N10" s="116" t="s">
+      <c r="N10" s="118"/>
+      <c r="O10" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="O10" s="118"/>
-      <c r="P10" s="101"/>
+      <c r="P10" s="118"/>
       <c r="Q10" s="101"/>
-    </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R10" s="101"/>
+    </row>
+    <row r="11" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="114">
         <v>42736</v>
       </c>
@@ -17833,14 +17960,15 @@
       </c>
       <c r="L11" s="118"/>
       <c r="M11" s="118"/>
-      <c r="N11" s="116" t="s">
+      <c r="N11" s="118"/>
+      <c r="O11" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="O11" s="118"/>
-      <c r="P11" s="101"/>
+      <c r="P11" s="118"/>
       <c r="Q11" s="101"/>
-    </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R11" s="101"/>
+    </row>
+    <row r="12" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9">
         <v>42736</v>
       </c>
@@ -17872,20 +18000,21 @@
       <c r="K12" s="101" t="s">
         <v>195</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3" t="s">
+      <c r="L12" s="101"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="9">
         <v>42736</v>
       </c>
@@ -17917,40 +18046,41 @@
       <c r="K13" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="3" t="s">
+      <c r="L13" s="101"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="9">
         <v>42736</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>212</v>
+      <c r="E14" s="116" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="122" t="s">
+        <v>317</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="3" t="s">
-        <v>81</v>
+      <c r="I14" s="122" t="s">
+        <v>316</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -17958,54 +18088,77 @@
       <c r="K14" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L14" s="4"/>
+      <c r="L14" s="162" t="s">
+        <v>319</v>
+      </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9">
+        <v>42736</v>
+      </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="4"/>
+      <c r="I15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="101" t="s">
+        <v>267</v>
+      </c>
+      <c r="L15" s="101"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="O15" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="122"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="122"/>
       <c r="J16" s="4"/>
       <c r="K16" s="101"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="160"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
@@ -18017,14 +18170,15 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="101"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="101"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4"/>
@@ -18036,17 +18190,18 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="101"/>
-      <c r="L18" s="4"/>
+      <c r="L18" s="101"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -18055,12 +18210,33 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="101"/>
-      <c r="L19" s="4"/>
+      <c r="L19" s="101"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -18086,7 +18262,7 @@
     <col min="3" max="3" width="29.8203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.8203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.17578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.29296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.3515625" style="1" customWidth="1"/>
     <col min="7" max="1025" width="8.8203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>